<commit_message>
izbrisani xlsx ki jih ne potrebujemo
</commit_message>
<xml_diff>
--- a/profili/001_data_vhodni_podatki_za_model_latest.xlsx
+++ b/profili/001_data_vhodni_podatki_za_model_latest.xlsx
@@ -2928,8 +2928,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008E7BE7B0CAABA43AED742E598976A4A" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5768611ea62c0e1bf83d4498f2411bf5">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7729c1d4-cef5-4d42-90b0-1acbf86e465b" xmlns:ns3="df635b4a-7af1-4a5e-a23a-fe7c9242efac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5936fe5d9f34e1640289d11b59618ac6" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010008E7BE7B0CAABA43AED742E598976A4A" ma:contentTypeVersion="19" ma:contentTypeDescription="Ustvari nov dokument." ma:contentTypeScope="" ma:versionID="0bdb3e7dd2ec873778367a96bf274037">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7729c1d4-cef5-4d42-90b0-1acbf86e465b" xmlns:ns3="df635b4a-7af1-4a5e-a23a-fe7c9242efac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dba111026cf164cdef25e61245610361" ns2:_="" ns3:_="">
     <xsd:import namespace="7729c1d4-cef5-4d42-90b0-1acbf86e465b"/>
     <xsd:import namespace="df635b4a-7af1-4a5e-a23a-fe7c9242efac"/>
     <xsd:element name="properties">
@@ -3025,7 +3025,7 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="b5c7bf33-a257-4e00-9403-561934745116" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Oznake slike" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="b5c7bf33-a257-4e00-9403-561934745116" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -3051,7 +3051,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="df635b4a-7af1-4a5e-a23a-fe7c9242efac" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="V skupni rabi z" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -3070,7 +3070,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="V skupni rabi s podrobnostmi" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -3098,8 +3098,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Vrsta vsebine"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Naslov"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -3208,20 +3208,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDCC0F2C-5D94-49E9-A7BA-4F24FDA1A6F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7729c1d4-cef5-4d42-90b0-1acbf86e465b"/>
-    <ds:schemaRef ds:uri="df635b4a-7af1-4a5e-a23a-fe7c9242efac"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC2258AD-74B5-4A55-8BC1-48BC7EF800EB}"/>
 </file>
</xml_diff>